<commit_message>
updated code and runtime
</commit_message>
<xml_diff>
--- a/Runtime_data.xlsx
+++ b/Runtime_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\HSG\Big Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8C27E9-94DD-45E6-B1A1-39823C9E9B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6148AF15-0033-46D3-9992-7CF1F27E1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{24E1C225-BDA7-4C13-8D5B-5CAD8935102D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{24E1C225-BDA7-4C13-8D5B-5CAD8935102D}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Original dataset</t>
   </si>
@@ -77,10 +77,22 @@
     <t>8.696434 min</t>
   </si>
   <si>
-    <t>R with optimisation</t>
-  </si>
-  <si>
     <t>3+ hours (N/A)</t>
+  </si>
+  <si>
+    <t>R with parallel processing</t>
+  </si>
+  <si>
+    <t>20.56177 sec</t>
+  </si>
+  <si>
+    <t>1.232462 min</t>
+  </si>
+  <si>
+    <t>3.706336 sec</t>
+  </si>
+  <si>
+    <t>1.159958 sec</t>
   </si>
 </sst>
 </file>
@@ -241,9 +253,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -253,18 +275,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -582,7 +592,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,406 +606,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2">
         <v>26</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>5052</v>
-      </c>
-      <c r="C3" s="7"/>
+      <c r="B3">
+        <v>5052</v>
+      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <f>B2*B3</f>
         <v>131352</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="8">
         <v>4</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="8">
         <v>5</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="8">
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="8">
         <v>7</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="8">
         <v>8</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="8">
         <v>9</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>351</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>2951</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>17901</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9">
         <v>83681</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="E10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="F10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="H10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="I10" s="6">
-        <v>5052</v>
-      </c>
-      <c r="J10" s="7">
+      <c r="B10">
+        <v>5052</v>
+      </c>
+      <c r="C10">
+        <v>5052</v>
+      </c>
+      <c r="D10">
+        <v>5052</v>
+      </c>
+      <c r="E10">
+        <v>5052</v>
+      </c>
+      <c r="F10">
+        <v>5052</v>
+      </c>
+      <c r="G10">
+        <v>5052</v>
+      </c>
+      <c r="H10">
+        <v>5052</v>
+      </c>
+      <c r="I10">
+        <v>5052</v>
+      </c>
+      <c r="J10" s="3">
         <v>5052</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
         <f>B9*B10</f>
         <v>1773252</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11">
         <f t="shared" ref="C11:J11" si="0">C9*C10</f>
         <v>14908452</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>90435852</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>422756412</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="5">
         <v>14.1</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="5">
         <v>114.8</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>694.1</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>3244.5</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
+      <c r="A16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="8">
         <v>2</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="8">
         <v>3</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="8">
         <v>4</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="8">
         <v>5</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="8">
         <v>6</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="8">
         <v>7</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <v>8</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="8">
         <v>9</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18">
         <v>351</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18">
         <v>2951</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>17901</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18">
         <v>83681</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="C19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="D19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="E19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="F19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="G19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="H19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="I19" s="6">
-        <v>5052</v>
-      </c>
-      <c r="J19" s="7">
+      <c r="B19">
+        <v>5052</v>
+      </c>
+      <c r="C19">
+        <v>5052</v>
+      </c>
+      <c r="D19">
+        <v>5052</v>
+      </c>
+      <c r="E19">
+        <v>5052</v>
+      </c>
+      <c r="F19">
+        <v>5052</v>
+      </c>
+      <c r="G19">
+        <v>5052</v>
+      </c>
+      <c r="H19">
+        <v>5052</v>
+      </c>
+      <c r="I19">
+        <v>5052</v>
+      </c>
+      <c r="J19" s="3">
         <v>5052</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20">
         <f>B18*B19</f>
         <v>1773252</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20">
         <f t="shared" ref="C20" si="1">C18*C19</f>
         <v>14908452</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20">
         <f t="shared" ref="D20" si="2">D18*D19</f>
         <v>90435852</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20">
         <f t="shared" ref="E20" si="3">E18*E19</f>
         <v>422756412</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20">
         <f t="shared" ref="F20" si="4">F18*F19</f>
         <v>0</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20">
         <f t="shared" ref="G20" si="5">G18*G19</f>
         <v>0</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20">
         <f t="shared" ref="H20" si="6">H18*H19</f>
         <v>0</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20">
         <f t="shared" ref="I20" si="7">I18*I19</f>
         <v>0</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="3">
         <f t="shared" ref="J20" si="8">J18*J19</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="7"/>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="5">
         <v>14.1</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="5">
         <v>114.8</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="5">
         <v>694.1</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>3244.5</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="10"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>